<commit_message>
Final version code from 23.06.2024 without pipeline base
</commit_message>
<xml_diff>
--- a/log-service/downloads_calendar/Calendar_7675.xlsx
+++ b/log-service/downloads_calendar/Calendar_7675.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="139">
   <si>
     <t>Календарный план</t>
   </si>
@@ -23,7 +23,7 @@
     <t>на выполнение проектных и изыскательских работ</t>
   </si>
   <si>
-    <t>Обустройство Байкаловского нефтегазоконденсатного месторождения. Инженерная подготовка кустовой площадки №1</t>
+    <t>Обустройство Байкаловского нефтегазоконденсатного месторождения. Обустройство кустовой площадки №2</t>
   </si>
   <si>
     <t>Шифр 7675</t>
@@ -68,10 +68,10 @@
     <t>Инженерные изыскания</t>
   </si>
   <si>
-    <t>05.06.2024</t>
-  </si>
-  <si>
-    <t>14.10.2024</t>
+    <t>24.06.2024</t>
+  </si>
+  <si>
+    <t>09.12.2024</t>
   </si>
   <si>
     <t>1.1</t>
@@ -80,7 +80,7 @@
     <t>Инженерные изыскания (полевые работы)</t>
   </si>
   <si>
-    <t>12.07.2024</t>
+    <t>03.09.2024</t>
   </si>
   <si>
     <t>1.2</t>
@@ -89,7 +89,10 @@
     <t xml:space="preserve">Инженерные изыскания (камеральные  работы) - выдача отчета (60% от общей стоимости камеральных работ) </t>
   </si>
   <si>
-    <t>13.08.2024</t>
+    <t>15.08.2024</t>
+  </si>
+  <si>
+    <t>18.10.2024</t>
   </si>
   <si>
     <t>1.3</t>
@@ -98,10 +101,28 @@
     <t>Инженерные изыскания (камеральные  работы) согласование отчета (40% от общей стоимости камеральных работ)</t>
   </si>
   <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>Инженерно-экологические изыскания</t>
+  </si>
+  <si>
+    <t>09.01.2025</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>Историко-культурные изыскания</t>
+  </si>
+  <si>
     <t>Рабочая документация</t>
   </si>
   <si>
-    <t>02.12.2024</t>
+    <t>09.10.2024</t>
+  </si>
+  <si>
+    <t>03.04.2025</t>
   </si>
   <si>
     <t>2.1</t>
@@ -110,16 +131,13 @@
     <t>Рабочая документация (60%, выдача документации ОГ)</t>
   </si>
   <si>
-    <t>03.09.2024</t>
-  </si>
-  <si>
     <t>2.2</t>
   </si>
   <si>
     <t>Рабочая документация (30%, согласование документации с ОГ и УВЭ)</t>
   </si>
   <si>
-    <t>05.11.2024</t>
+    <t>03.03.2025</t>
   </si>
   <si>
     <t>2.3</t>
@@ -128,7 +146,10 @@
     <t>Рабочая документация  (5%, выдача сметной документации ОГ)</t>
   </si>
   <si>
-    <t>02.10.2024</t>
+    <t>23.12.2024</t>
+  </si>
+  <si>
+    <t>07.02.2025</t>
   </si>
   <si>
     <t>2.4</t>
@@ -140,46 +161,271 @@
     <t>Проектная документация</t>
   </si>
   <si>
+    <t>01.09.2025</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>Проектная документация (60%, выдача документации ОГ)</t>
+  </si>
+  <si>
+    <t>11.02.2025</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>Проектная документация (20%, согласование документации с ОГ и УВЭ)</t>
+  </si>
+  <si>
+    <t>02.05.2025</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>Проектная документация (20%, проведение внешних экспертиз)</t>
+  </si>
+  <si>
+    <t>Землеустроительные работы</t>
+  </si>
+  <si>
+    <t>09.07.2025</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>Землеустроительная документация</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Прочие работы</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>Проект санитарно-защитных зон промышленного объекта</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>Разработка рыбохозяйственного раздела</t>
+  </si>
+  <si>
+    <t>20.06.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ИТОГО: </t>
+  </si>
+  <si>
+    <t>Этап строительства 2</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>03.06.2025</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>14.01.2025</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>26.12.2024</t>
+  </si>
+  <si>
     <t>02.04.2025</t>
   </si>
   <si>
-    <t>3.1</t>
-  </si>
-  <si>
-    <t>Проектная документация (60%, выдача документации ОГ)</t>
-  </si>
-  <si>
-    <t>04.10.2024</t>
-  </si>
-  <si>
-    <t>3.2</t>
-  </si>
-  <si>
-    <t>Проектная документация (20%, согласование документации с ОГ и УВЭ)</t>
-  </si>
-  <si>
-    <t>03.12.2024</t>
-  </si>
-  <si>
-    <t>3.3</t>
-  </si>
-  <si>
-    <t>Проектная документация (20%, проведение внешних экспертиз)</t>
-  </si>
-  <si>
-    <t>Землеустроительные работы</t>
-  </si>
-  <si>
-    <t>03.02.2025</t>
-  </si>
-  <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>Землеустроительная документация</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ИТОГО: </t>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>24.03.2025</t>
+  </si>
+  <si>
+    <t>11.08.2025</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>14.07.2025</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>14.05.2025</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>03.02.2026</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>17.07.2025</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>06.10.2025</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>09.01.2026</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t>03.12.2025</t>
+  </si>
+  <si>
+    <t>Этап строительства 3</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>02.06.2025</t>
+  </si>
+  <si>
+    <t>11.1</t>
+  </si>
+  <si>
+    <t>05.03.2025</t>
+  </si>
+  <si>
+    <t>11.2</t>
+  </si>
+  <si>
+    <t>28.02.2025</t>
+  </si>
+  <si>
+    <t>14.04.2025</t>
+  </si>
+  <si>
+    <t>11.3</t>
+  </si>
+  <si>
+    <t>11.4</t>
+  </si>
+  <si>
+    <t>11.5</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>09.09.2025</t>
+  </si>
+  <si>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t>13.05.2025</t>
+  </si>
+  <si>
+    <t>12.2</t>
+  </si>
+  <si>
+    <t>03.07.2025</t>
+  </si>
+  <si>
+    <t>12.3</t>
+  </si>
+  <si>
+    <t>10.06.2025</t>
+  </si>
+  <si>
+    <t>04.08.2025</t>
+  </si>
+  <si>
+    <t>12.4</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>13.01.2026</t>
+  </si>
+  <si>
+    <t>13.1</t>
+  </si>
+  <si>
+    <t>30.04.2025</t>
+  </si>
+  <si>
+    <t>13.2</t>
+  </si>
+  <si>
+    <t>15.09.2025</t>
+  </si>
+  <si>
+    <t>13.3</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>15.1</t>
+  </si>
+  <si>
+    <t>15.2</t>
+  </si>
+  <si>
+    <t>03.11.2025</t>
   </si>
   <si>
     <t xml:space="preserve">ВСЕГО по договору: </t>
@@ -302,7 +548,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A4:D33"/>
+  <dimension ref="A4:D84"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -461,80 +707,80 @@
         <v>24</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" ht="42.0" customHeight="true">
       <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" ht="33.0" customHeight="true">
-      <c r="A20" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="6" t="s">
+    <row r="20" ht="42.0" customHeight="true">
+      <c r="A20" s="4" t="s">
         <v>29</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="21" ht="42.0" customHeight="true">
       <c r="A21" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" ht="42.0" customHeight="true">
-      <c r="A22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="5" t="s">
+    </row>
+    <row r="22" ht="33.0" customHeight="true">
+      <c r="A22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="6" t="s">
         <v>35</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="23" ht="42.0" customHeight="true">
       <c r="A23" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" ht="42.0" customHeight="true">
@@ -545,130 +791,816 @@
         <v>40</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" ht="33.0" customHeight="true">
-      <c r="A25" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="6" t="s">
+    </row>
+    <row r="25" ht="42.0" customHeight="true">
+      <c r="A25" s="4" t="s">
         <v>42</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" ht="42.0" customHeight="true">
       <c r="A26" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" ht="42.0" customHeight="true">
-      <c r="A27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" ht="33.0" customHeight="true">
+      <c r="A27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>48</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="28" ht="42.0" customHeight="true">
       <c r="A28" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" ht="33.0" customHeight="true">
-      <c r="A29" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="6" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="29" ht="42.0" customHeight="true">
+      <c r="A29" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="30" ht="42.0" customHeight="true">
       <c r="A30" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" ht="33.0" customHeight="true">
       <c r="A31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" ht="42.0" customHeight="true">
+      <c r="A32" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" ht="33.0" customHeight="true">
+      <c r="A33" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" ht="42.0" customHeight="true">
+      <c r="A34" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" ht="42.0" customHeight="true">
+      <c r="A35" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" ht="33.0" customHeight="true">
+      <c r="A36" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="B36" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" ht="15.0" customHeight="true">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" ht="33.0" customHeight="true">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="D36" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" ht="15.0" customHeight="true">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" ht="27.0" customHeight="true">
+      <c r="A38" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" ht="33.0" customHeight="true">
+      <c r="A39" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" ht="42.0" customHeight="true">
+      <c r="A40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" ht="42.0" customHeight="true">
+      <c r="A41" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" ht="42.0" customHeight="true">
+      <c r="A42" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" ht="42.0" customHeight="true">
+      <c r="A43" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>42</v>
+      <c r="D43" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" ht="42.0" customHeight="true">
+      <c r="A44" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" ht="33.0" customHeight="true">
+      <c r="A45" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" ht="42.0" customHeight="true">
+      <c r="A46" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" ht="42.0" customHeight="true">
+      <c r="A47" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" ht="42.0" customHeight="true">
+      <c r="A48" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" ht="42.0" customHeight="true">
+      <c r="A49" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" ht="33.0" customHeight="true">
+      <c r="A50" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" ht="42.0" customHeight="true">
+      <c r="A51" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" ht="42.0" customHeight="true">
+      <c r="A52" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" ht="42.0" customHeight="true">
+      <c r="A53" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" ht="33.0" customHeight="true">
+      <c r="A54" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" ht="42.0" customHeight="true">
+      <c r="A55" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" ht="33.0" customHeight="true">
+      <c r="A56" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" ht="42.0" customHeight="true">
+      <c r="A57" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" ht="42.0" customHeight="true">
+      <c r="A58" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" ht="33.0" customHeight="true">
+      <c r="A59" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" ht="15.0" customHeight="true">
+      <c r="A60" s="4"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" ht="27.0" customHeight="true">
+      <c r="A61" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B61" s="7"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+    </row>
+    <row r="62" ht="33.0" customHeight="true">
+      <c r="A62" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" ht="42.0" customHeight="true">
+      <c r="A63" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" ht="42.0" customHeight="true">
+      <c r="A64" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" ht="42.0" customHeight="true">
+      <c r="A65" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" ht="42.0" customHeight="true">
+      <c r="A66" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" ht="42.0" customHeight="true">
+      <c r="A67" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" ht="33.0" customHeight="true">
+      <c r="A68" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" ht="42.0" customHeight="true">
+      <c r="A69" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" ht="42.0" customHeight="true">
+      <c r="A70" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" ht="42.0" customHeight="true">
+      <c r="A71" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" ht="42.0" customHeight="true">
+      <c r="A72" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" ht="33.0" customHeight="true">
+      <c r="A73" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" ht="42.0" customHeight="true">
+      <c r="A74" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="75" ht="42.0" customHeight="true">
+      <c r="A75" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="76" ht="42.0" customHeight="true">
+      <c r="A76" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="77" ht="33.0" customHeight="true">
+      <c r="A77" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" ht="42.0" customHeight="true">
+      <c r="A78" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79" ht="33.0" customHeight="true">
+      <c r="A79" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="80" ht="42.0" customHeight="true">
+      <c r="A80" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="81" ht="42.0" customHeight="true">
+      <c r="A81" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="82" ht="33.0" customHeight="true">
+      <c r="A82" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="83" ht="15.0" customHeight="true">
+      <c r="A83" s="4"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+    </row>
+    <row r="84" ht="33.0" customHeight="true">
+      <c r="A84" s="6"/>
+      <c r="B84" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="15">
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A6:D6"/>
@@ -679,7 +1611,11 @@
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A83:D83"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Final version code from 02.07.2024 with full test base
</commit_message>
<xml_diff>
--- a/log-service/downloads_calendar/Calendar_7675.xlsx
+++ b/log-service/downloads_calendar/Calendar_7675.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="141">
   <si>
     <t>Календарный план</t>
   </si>
@@ -23,7 +23,7 @@
     <t>на выполнение проектных и изыскательских работ</t>
   </si>
   <si>
-    <t>Обустройство Байкаловского нефтегазоконденсатного месторождения. Обустройство кустовой площадки №2</t>
+    <t>Обустройство Байкаловского нефтегазоконденсатного месторождения. Инженерная подготовка кустовой площадки №1</t>
   </si>
   <si>
     <t>Шифр 7675</t>
@@ -68,10 +68,10 @@
     <t>Инженерные изыскания</t>
   </si>
   <si>
-    <t>24.06.2024</t>
-  </si>
-  <si>
-    <t>09.12.2024</t>
+    <t>02.07.2024</t>
+  </si>
+  <si>
+    <t>10.06.2025</t>
   </si>
   <si>
     <t>1.1</t>
@@ -80,7 +80,7 @@
     <t>Инженерные изыскания (полевые работы)</t>
   </si>
   <si>
-    <t>03.09.2024</t>
+    <t>13.02.2025</t>
   </si>
   <si>
     <t>1.2</t>
@@ -89,10 +89,10 @@
     <t xml:space="preserve">Инженерные изыскания (камеральные  работы) - выдача отчета (60% от общей стоимости камеральных работ) </t>
   </si>
   <si>
-    <t>15.08.2024</t>
-  </si>
-  <si>
-    <t>18.10.2024</t>
+    <t>04.02.2025</t>
+  </si>
+  <si>
+    <t>05.05.2025</t>
   </si>
   <si>
     <t>1.3</t>
@@ -119,10 +119,10 @@
     <t>Рабочая документация</t>
   </si>
   <si>
-    <t>09.10.2024</t>
-  </si>
-  <si>
-    <t>03.04.2025</t>
+    <t>11.04.2025</t>
+  </si>
+  <si>
+    <t>03.10.2025</t>
   </si>
   <si>
     <t>2.1</t>
@@ -131,13 +131,16 @@
     <t>Рабочая документация (60%, выдача документации ОГ)</t>
   </si>
   <si>
+    <t>11.07.2025</t>
+  </si>
+  <si>
     <t>2.2</t>
   </si>
   <si>
     <t>Рабочая документация (30%, согласование документации с ОГ и УВЭ)</t>
   </si>
   <si>
-    <t>03.03.2025</t>
+    <t>01.09.2025</t>
   </si>
   <si>
     <t>2.3</t>
@@ -146,10 +149,10 @@
     <t>Рабочая документация  (5%, выдача сметной документации ОГ)</t>
   </si>
   <si>
-    <t>23.12.2024</t>
-  </si>
-  <si>
-    <t>07.02.2025</t>
+    <t>02.07.2025</t>
+  </si>
+  <si>
+    <t>11.08.2025</t>
   </si>
   <si>
     <t>2.4</t>
@@ -161,7 +164,7 @@
     <t>Проектная документация</t>
   </si>
   <si>
-    <t>01.09.2025</t>
+    <t>18.03.2026</t>
   </si>
   <si>
     <t>3.1</t>
@@ -170,7 +173,7 @@
     <t>Проектная документация (60%, выдача документации ОГ)</t>
   </si>
   <si>
-    <t>11.02.2025</t>
+    <t>03.09.2025</t>
   </si>
   <si>
     <t>3.2</t>
@@ -179,7 +182,7 @@
     <t>Проектная документация (20%, согласование документации с ОГ и УВЭ)</t>
   </si>
   <si>
-    <t>02.05.2025</t>
+    <t>18.11.2025</t>
   </si>
   <si>
     <t>3.3</t>
@@ -191,7 +194,7 @@
     <t>Землеустроительные работы</t>
   </si>
   <si>
-    <t>09.07.2025</t>
+    <t>03.02.2026</t>
   </si>
   <si>
     <t>4.1</t>
@@ -218,7 +221,7 @@
     <t>Разработка рыбохозяйственного раздела</t>
   </si>
   <si>
-    <t>20.06.2025</t>
+    <t>13.01.2026</t>
   </si>
   <si>
     <t xml:space="preserve">ИТОГО: </t>
@@ -230,22 +233,19 @@
     <t>6</t>
   </si>
   <si>
-    <t>03.06.2025</t>
-  </si>
-  <si>
     <t>6.1</t>
   </si>
   <si>
-    <t>14.01.2025</t>
+    <t>16.10.2025</t>
   </si>
   <si>
     <t>6.2</t>
   </si>
   <si>
-    <t>26.12.2024</t>
-  </si>
-  <si>
-    <t>02.04.2025</t>
+    <t>07.10.2025</t>
+  </si>
+  <si>
+    <t>04.12.2025</t>
   </si>
   <si>
     <t>6.3</t>
@@ -260,25 +260,28 @@
     <t>7</t>
   </si>
   <si>
-    <t>24.03.2025</t>
-  </si>
-  <si>
-    <t>11.08.2025</t>
+    <t>25.11.2025</t>
+  </si>
+  <si>
+    <t>05.05.2026</t>
   </si>
   <si>
     <t>7.1</t>
   </si>
   <si>
+    <t>12.02.2026</t>
+  </si>
+  <si>
     <t>7.2</t>
   </si>
   <si>
-    <t>14.07.2025</t>
+    <t>06.04.2026</t>
   </si>
   <si>
     <t>7.3</t>
   </si>
   <si>
-    <t>14.05.2025</t>
+    <t>17.03.2026</t>
   </si>
   <si>
     <t>7.4</t>
@@ -287,19 +290,19 @@
     <t>8</t>
   </si>
   <si>
-    <t>03.02.2026</t>
+    <t>14.10.2026</t>
   </si>
   <si>
     <t>8.1</t>
   </si>
   <si>
-    <t>17.07.2025</t>
+    <t>03.04.2026</t>
   </si>
   <si>
     <t>8.2</t>
   </si>
   <si>
-    <t>06.10.2025</t>
+    <t>16.06.2026</t>
   </si>
   <si>
     <t>8.3</t>
@@ -308,46 +311,46 @@
     <t>9</t>
   </si>
   <si>
+    <t>03.09.2026</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t>04.08.2026</t>
+  </si>
+  <si>
+    <t>Этап строительства 3</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>14.04.2026</t>
+  </si>
+  <si>
+    <t>11.1</t>
+  </si>
+  <si>
     <t>09.01.2026</t>
   </si>
   <si>
-    <t>9.1</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>10.1</t>
-  </si>
-  <si>
-    <t>10.2</t>
-  </si>
-  <si>
-    <t>03.12.2025</t>
-  </si>
-  <si>
-    <t>Этап строительства 3</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>02.06.2025</t>
-  </si>
-  <si>
-    <t>11.1</t>
-  </si>
-  <si>
-    <t>05.03.2025</t>
-  </si>
-  <si>
     <t>11.2</t>
   </si>
   <si>
-    <t>28.02.2025</t>
-  </si>
-  <si>
-    <t>14.04.2025</t>
+    <t>17.12.2025</t>
+  </si>
+  <si>
+    <t>03.03.2026</t>
   </si>
   <si>
     <t>11.3</t>
@@ -362,28 +365,31 @@
     <t>12</t>
   </si>
   <si>
-    <t>09.09.2025</t>
+    <t>13.02.2026</t>
+  </si>
+  <si>
+    <t>02.11.2026</t>
   </si>
   <si>
     <t>12.1</t>
   </si>
   <si>
-    <t>13.05.2025</t>
+    <t>15.07.2026</t>
   </si>
   <si>
     <t>12.2</t>
   </si>
   <si>
-    <t>03.07.2025</t>
+    <t>04.09.2026</t>
   </si>
   <si>
     <t>12.3</t>
   </si>
   <si>
-    <t>10.06.2025</t>
-  </si>
-  <si>
-    <t>04.08.2025</t>
+    <t>06.07.2026</t>
+  </si>
+  <si>
+    <t>11.09.2026</t>
   </si>
   <si>
     <t>12.4</t>
@@ -392,19 +398,16 @@
     <t>13</t>
   </si>
   <si>
-    <t>13.01.2026</t>
+    <t>12.03.2027</t>
   </si>
   <si>
     <t>13.1</t>
   </si>
   <si>
-    <t>30.04.2025</t>
-  </si>
-  <si>
     <t>13.2</t>
   </si>
   <si>
-    <t>15.09.2025</t>
+    <t>12.11.2026</t>
   </si>
   <si>
     <t>13.3</t>
@@ -413,6 +416,9 @@
     <t>14</t>
   </si>
   <si>
+    <t>20.01.2027</t>
+  </si>
+  <si>
     <t>14.1</t>
   </si>
   <si>
@@ -425,7 +431,7 @@
     <t>15.2</t>
   </si>
   <si>
-    <t>03.11.2025</t>
+    <t>11.01.2027</t>
   </si>
   <si>
     <t xml:space="preserve">ВСЕГО по договору: </t>
@@ -780,43 +786,43 @@
         <v>35</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" ht="42.0" customHeight="true">
       <c r="A24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="D24" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" ht="42.0" customHeight="true">
       <c r="A25" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" ht="42.0" customHeight="true">
       <c r="A26" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>26</v>
@@ -830,55 +836,55 @@
         <v>14</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" ht="42.0" customHeight="true">
       <c r="A28" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" ht="42.0" customHeight="true">
       <c r="A29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" ht="42.0" customHeight="true">
       <c r="A30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="D30" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" ht="33.0" customHeight="true">
@@ -886,69 +892,69 @@
         <v>15</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" ht="42.0" customHeight="true">
       <c r="A32" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="33" ht="33.0" customHeight="true">
       <c r="A33" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" ht="42.0" customHeight="true">
       <c r="A34" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" ht="42.0" customHeight="true">
       <c r="A35" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" ht="33.0" customHeight="true">
@@ -956,13 +962,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" ht="15.0" customHeight="true">
@@ -973,7 +979,7 @@
     </row>
     <row r="38" ht="27.0" customHeight="true">
       <c r="A38" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="6"/>
@@ -981,7 +987,7 @@
     </row>
     <row r="39" ht="33.0" customHeight="true">
       <c r="A39" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>17</v>
@@ -990,7 +996,7 @@
         <v>25</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" ht="42.0" customHeight="true">
@@ -1032,7 +1038,7 @@
         <v>77</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" ht="42.0" customHeight="true">
@@ -1088,43 +1094,43 @@
         <v>82</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" ht="42.0" customHeight="true">
       <c r="A47" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="D47" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" ht="42.0" customHeight="true">
       <c r="A48" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" ht="42.0" customHeight="true">
       <c r="A49" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>77</v>
@@ -1135,128 +1141,128 @@
     </row>
     <row r="50" ht="33.0" customHeight="true">
       <c r="A50" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" ht="42.0" customHeight="true">
       <c r="A51" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" ht="42.0" customHeight="true">
       <c r="A52" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="D52" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" ht="42.0" customHeight="true">
       <c r="A53" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="D53" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" ht="33.0" customHeight="true">
       <c r="A54" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" ht="42.0" customHeight="true">
       <c r="A55" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="56" ht="33.0" customHeight="true">
       <c r="A56" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" ht="42.0" customHeight="true">
       <c r="A57" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" ht="42.0" customHeight="true">
       <c r="A58" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" ht="33.0" customHeight="true">
@@ -1264,13 +1270,13 @@
         <v>1</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" ht="15.0" customHeight="true">
@@ -1281,7 +1287,7 @@
     </row>
     <row r="61" ht="27.0" customHeight="true">
       <c r="A61" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="6"/>
@@ -1289,7 +1295,7 @@
     </row>
     <row r="62" ht="33.0" customHeight="true">
       <c r="A62" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>17</v>
@@ -1298,12 +1304,12 @@
         <v>76</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="63" ht="42.0" customHeight="true">
       <c r="A63" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>21</v>
@@ -1312,40 +1318,40 @@
         <v>76</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="64" ht="42.0" customHeight="true">
       <c r="A64" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" ht="42.0" customHeight="true">
       <c r="A65" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" ht="42.0" customHeight="true">
       <c r="A66" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>30</v>
@@ -1359,7 +1365,7 @@
     </row>
     <row r="67" ht="42.0" customHeight="true">
       <c r="A67" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>33</v>
@@ -1373,198 +1379,198 @@
     </row>
     <row r="68" ht="33.0" customHeight="true">
       <c r="A68" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>36</v>
+        <v>117</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" ht="42.0" customHeight="true">
       <c r="A69" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>36</v>
+        <v>117</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" ht="42.0" customHeight="true">
       <c r="A70" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" ht="42.0" customHeight="true">
       <c r="A71" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="72" ht="42.0" customHeight="true">
       <c r="A72" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" ht="33.0" customHeight="true">
       <c r="A73" s="6" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="74" ht="42.0" customHeight="true">
       <c r="A74" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" ht="42.0" customHeight="true">
       <c r="A75" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" ht="42.0" customHeight="true">
       <c r="A76" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C76" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="D76" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="77" ht="33.0" customHeight="true">
       <c r="A77" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" ht="42.0" customHeight="true">
       <c r="A78" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" ht="33.0" customHeight="true">
       <c r="A79" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D79" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="80" ht="42.0" customHeight="true">
       <c r="A80" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" ht="42.0" customHeight="true">
       <c r="A81" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" ht="33.0" customHeight="true">
@@ -1572,13 +1578,13 @@
         <v>1</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>76</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="83" ht="15.0" customHeight="true">
@@ -1590,13 +1596,13 @@
     <row r="84" ht="33.0" customHeight="true">
       <c r="A84" s="6"/>
       <c r="B84" s="7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>